<commit_message>
Added reference to dataset
</commit_message>
<xml_diff>
--- a/data/data_matlab.xlsx
+++ b/data/data_matlab.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/psoriasis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/npz3/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD622DD-397F-4D46-98CC-957C622A8195}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA2228B-A66D-524A-A688-B769BA0850B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35860" yWindow="500" windowWidth="37800" windowHeight="21780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8540" yWindow="1800" windowWidth="35360" windowHeight="20820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Reference" sheetId="2" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="144">
   <si>
     <t>LAST_FU_PASI</t>
   </si>
@@ -451,12 +450,37 @@
   <si>
     <t>UVB_DOSE_33</t>
   </si>
+  <si>
+    <t>https://doi.org/10.1111/jdv.17519</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>The use of psoriasis biomarkers, including trajectory of clinical response, to predict clearance and remission duration to UVB phototherapy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. N. Watson, N. Wilson, F. Shmarov, P. Zuliani, N. J. Reynolds, S. C. Weatherhead. Journal of the European Academy of Dermatology &amp; Venereology 35: 2250-2258, 2021.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If you use this dataset in a publication, please cite:  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -524,6 +548,31 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -549,10 +598,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -577,8 +627,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -958,10 +1019,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6E4E1C-B2D6-B444-9B6A-3E256150DA93}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="102.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+    </row>
+    <row r="3" spans="1:1" ht="88" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{79260DA5-26FA-9A47-82D2-E93B3815E76E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GC445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
@@ -14660,32 +14763,4 @@
   <pageMargins left="0.74791666666667" right="0.74791666666667" top="0.98402777777778005" bottom="0.98402777777778005" header="0.51180555555554996" footer="0.51180555555554996"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.74791666666667" right="0.74791666666667" top="0.98402777777778005" bottom="0.98402777777778005" header="0.51180555555554996" footer="0.51180555555554996"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.74791666666667" right="0.74791666666667" top="0.98402777777778005" bottom="0.98402777777778005" header="0.51180555555554996" footer="0.51180555555554996"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
 </file>
</xml_diff>